<commit_message>
Add 90day support, improved transaction history container and retest
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randy/Documents/projects/hazelcast-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAB0BC0-B416-9D43-B678-9294E39513C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81EF0BC-4805-9449-A55C-1073FDF55B9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{63738722-5818-8F43-B05D-9165230C02A6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{63738722-5818-8F43-B05D-9165230C02A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,14 @@
     <sheet name="Base" sheetId="3" r:id="rId3"/>
     <sheet name="EP Pipeline" sheetId="4" r:id="rId4"/>
     <sheet name="EP Pipelining and Network Batch" sheetId="5" r:id="rId5"/>
+    <sheet name="+ 90 Day" sheetId="9" r:id="rId6"/>
+    <sheet name="+HD" sheetId="10" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$4:$A$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$3</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$4:$H$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nodes</t>
   </si>
@@ -56,6 +63,12 @@
   </si>
   <si>
     <t>Base +EP Pipelining and Network Batching</t>
+  </si>
+  <si>
+    <t>+90 Day + Improved History Data Structure</t>
+  </si>
+  <si>
+    <t>+HD</t>
   </si>
 </sst>
 </file>
@@ -342,29 +355,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -372,23 +388,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>116</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
@@ -549,29 +565,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -579,20 +598,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$10</c:f>
+              <c:f>Sheet1!$E$4:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>138</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>166</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>170</c:v>
                 </c:pt>
               </c:numCache>
@@ -753,29 +772,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -783,20 +805,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$10</c:f>
+              <c:f>Sheet1!$F$4:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>115</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>141</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>161</c:v>
                 </c:pt>
               </c:numCache>
@@ -949,29 +971,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -979,17 +1004,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$10</c:f>
+              <c:f>Sheet1!$G$4:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>193</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>267</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>323</c:v>
                 </c:pt>
               </c:numCache>
@@ -1531,29 +1556,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -1561,23 +1589,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>113</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>116</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
@@ -2092,29 +2120,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2122,20 +2153,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$10</c:f>
+              <c:f>Sheet1!$E$4:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>138</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>166</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>170</c:v>
                 </c:pt>
               </c:numCache>
@@ -2651,29 +2682,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$10</c:f>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2681,17 +2715,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$10</c:f>
+              <c:f>Sheet1!$G$4:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>193</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>267</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>323</c:v>
                 </c:pt>
               </c:numCache>
@@ -3005,6 +3039,524 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>+90 Day + Improved History Data Structure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3438420772116129E-2"/>
+                  <c:y val="-5.3876151916341691E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B77-1F48-9B5D-AC7C92FF5206}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1957911295"/>
+        <c:axId val="1957912975"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1957911295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Servers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1957912975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1957912975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Throughput K TPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1957911295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3165,6 +3717,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4714,6 +5306,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5393,10 +6501,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>730250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7C6D06-716D-304A-A6E1-B8DDA9A295F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3D20F78-20E5-8945-86AB-2E178E27CBF8}" name="Table1" displayName="Table1" ref="A3:G10" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A3:G10" xr:uid="{EDB8E479-5060-844C-9C4F-433171887051}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3D20F78-20E5-8945-86AB-2E178E27CBF8}" name="Table1" displayName="Table1" ref="A3:I11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A3:I11" xr:uid="{EDB8E479-5060-844C-9C4F-433171887051}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{850378A9-916D-9743-A391-DA2DB195DC4D}" name="Nodes"/>
     <tableColumn id="2" xr3:uid="{44000FEA-37D2-6B41-A950-419387013D48}" name="Base Architecture"/>
     <tableColumn id="3" xr3:uid="{00FFC7F8-3A55-9C49-A6E3-EF057D0C74B6}" name="Base + 1031 partitions and 128 readers"/>
@@ -5404,6 +6553,8 @@
     <tableColumn id="5" xr3:uid="{9BF17F3C-6490-C344-A308-4F4860596DB2}" name="Base + EP Pipelining"/>
     <tableColumn id="6" xr3:uid="{C645D1DC-3CE7-DE4F-94AF-C08440120BA5}" name="Base +Network Batching"/>
     <tableColumn id="7" xr3:uid="{57F19D1A-1EAC-AE47-AAA9-2BF09DEB516A}" name="Base +EP Pipelining and Network Batching"/>
+    <tableColumn id="8" xr3:uid="{46D98D51-992C-5448-9402-7F341FF10079}" name="+90 Day + Improved History Data Structure"/>
+    <tableColumn id="9" xr3:uid="{93D91894-C423-8F42-BEC3-4092D062D2F1}" name="+HD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5709,30 +6860,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5754,99 +6907,125 @@
       <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>232</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>102</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>138</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>97</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>124</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>156</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>115</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>267</v>
       </c>
+      <c r="H7">
+        <v>442</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>14</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>138</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>140</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>153</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>166</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>141</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>18</v>
       </c>
+      <c r="H10">
+        <v>663</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>20</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="E10">
+      <c r="C11" s="1"/>
+      <c r="E11">
         <v>170</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5906,7 +7085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4CD218-1F72-2A42-9781-EDC5D69950BD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5915,4 +7094,31 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC56A2B-6DAD-0B4C-A2C1-FE629ABB636E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A741B922-6C78-2E4F-8198-27EE63803883}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Run tests using HD.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randy/Documents/projects/hazelcast-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81EF0BC-4805-9449-A55C-1073FDF55B9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF6658-D56A-3847-8B37-8C5C21CB1118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{63738722-5818-8F43-B05D-9165230C02A6}"/>
   </bookViews>
@@ -21,11 +21,6 @@
     <sheet name="+ 90 Day" sheetId="9" r:id="rId6"/>
     <sheet name="+HD" sheetId="10" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$4:$A$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$4:$H$10</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3274,13 +3269,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>232</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>442</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>663</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3557,6 +3552,559 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>+HD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12960500963391136"/>
+                  <c:y val="-3.9690987367586243E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$4:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6B06-9F44-802E-5F4020338F7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1952126559"/>
+        <c:axId val="1951938735"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1952126559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Servers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1951938735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1951938735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>K TPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1952126559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3757,6 +4305,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5822,6 +6410,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6542,6 +7646,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E220478F-4034-DA43-917F-7D11DDE6F2C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3D20F78-20E5-8945-86AB-2E178E27CBF8}" name="Table1" displayName="Table1" ref="A3:I11" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:I11" xr:uid="{EDB8E479-5060-844C-9C4F-433171887051}"/>
@@ -6863,7 +8008,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6885,7 +8030,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -6924,9 +8069,11 @@
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
-        <v>232</v>
+        <v>183</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3">
+        <v>136</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -6970,7 +8117,10 @@
         <v>267</v>
       </c>
       <c r="H7">
-        <v>442</v>
+        <v>450</v>
+      </c>
+      <c r="I7">
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7009,7 +8159,10 @@
         <v>18</v>
       </c>
       <c r="H10">
-        <v>663</v>
+        <v>670</v>
+      </c>
+      <c r="I10">
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -7101,7 +8254,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7115,10 +8268,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A741B922-6C78-2E4F-8198-27EE63803883}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final commit for second submission.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randy/Documents/projects/hazelcast-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF6658-D56A-3847-8B37-8C5C21CB1118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEE7751-59BE-5B4B-BFC3-9946061ED152}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{63738722-5818-8F43-B05D-9165230C02A6}"/>
   </bookViews>
@@ -8008,7 +8008,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>